<commit_message>
adding citypop playlist to tracker
</commit_message>
<xml_diff>
--- a/playlists.xlsx
+++ b/playlists.xlsx
@@ -9,8 +9,8 @@
     <sheet name="playlists" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">playlists!$A$1:$D$1145</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">playlists!$A$1:$D$1214</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">playlists!$A$1:$D$1215</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">playlists!$A$1:$D$1215</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="2308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="2343">
   <si>
     <t xml:space="preserve">Playlist Name</t>
   </si>
@@ -6944,6 +6944,111 @@
   </si>
   <si>
     <t>Anti-Matter</t>
+  </si>
+  <si>
+    <t>CityPop</t>
+  </si>
+  <si>
+    <t>Fantasy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meiko Nakahara</t>
+  </si>
+  <si>
+    <t>じゃじゃ馬娘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taehko ohnuki</t>
+  </si>
+  <si>
+    <t>Wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miki Matsubara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit In Summer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omega Tribe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telephone number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just a Joke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yurie Kokubu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dress Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaoru Akimoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flyday Chinatown</t>
+  </si>
+  <si>
+    <t>Yasuha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shiny Lady</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiroshi Sato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stardust Night</t>
+  </si>
+  <si>
+    <t>Jadoes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simple Love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokyo Reggie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masayoshi Takanaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dolphin in Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kingo Hamada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Space Scraper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toshiki Kadomatsu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taeko Ohnuki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAY CITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Junko Yagami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hitonatsu no Tapestry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mystical Composer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kikuchi Momoko</t>
+  </si>
+  <si>
+    <t>Kagerou</t>
+  </si>
+  <si>
+    <t>Char</t>
   </si>
 </sst>
 </file>
@@ -7056,7 +7161,9 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="18" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7569,14 +7676,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A1179" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A325" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col bestFit="1" customWidth="1" min="1" max="1" style="0" width="28.7109375"/>
-    <col customWidth="1" min="2" max="2" style="0" width="85.28125"/>
+    <col customWidth="1" min="2" max="2" style="0" width="45.8515625"/>
     <col customWidth="1" min="3" max="3" style="0" width="43.285714285714299"/>
     <col customWidth="1" min="4" max="4" style="0" width="122.428571428571"/>
     <col min="5" max="16384" style="0" width="9.140625"/>
@@ -12418,7 +12525,7 @@
       <c r="E305"/>
       <c r="H305"/>
     </row>
-    <row r="306" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="306" s="5" customFormat="1" ht="12.75">
       <c r="A306" t="s">
         <v>632</v>
       </c>
@@ -12434,7 +12541,7 @@
       <c r="E306"/>
       <c r="H306"/>
     </row>
-    <row r="307" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="307" s="0" customFormat="1" ht="12.75">
       <c r="A307" t="s">
         <v>632</v>
       </c>
@@ -12450,7 +12557,7 @@
       <c r="E307"/>
       <c r="H307"/>
     </row>
-    <row r="308" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="308" s="5" customFormat="1" ht="12.75">
       <c r="A308" t="s">
         <v>632</v>
       </c>
@@ -12466,7 +12573,7 @@
       <c r="E308"/>
       <c r="H308"/>
     </row>
-    <row r="309" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="309" s="0" customFormat="1" ht="12.75">
       <c r="A309" t="s">
         <v>632</v>
       </c>
@@ -12482,7 +12589,7 @@
       <c r="E309"/>
       <c r="H309"/>
     </row>
-    <row r="310" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="310" s="5" customFormat="1" ht="12.75">
       <c r="A310" t="s">
         <v>632</v>
       </c>
@@ -12498,7 +12605,7 @@
       <c r="E310"/>
       <c r="H310"/>
     </row>
-    <row r="311" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="311" s="0" customFormat="1" ht="12.75">
       <c r="A311" t="s">
         <v>632</v>
       </c>
@@ -12514,7 +12621,7 @@
       <c r="E311"/>
       <c r="H311"/>
     </row>
-    <row r="312" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="312" s="5" customFormat="1" ht="12.75">
       <c r="A312" t="s">
         <v>632</v>
       </c>
@@ -12530,7 +12637,7 @@
       <c r="E312"/>
       <c r="H312"/>
     </row>
-    <row r="313" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="313" s="0" customFormat="1" ht="12.75">
       <c r="A313" t="s">
         <v>632</v>
       </c>
@@ -12546,7 +12653,7 @@
       <c r="E313"/>
       <c r="H313"/>
     </row>
-    <row r="314" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="314" s="5" customFormat="1" ht="12.75">
       <c r="A314" t="s">
         <v>632</v>
       </c>
@@ -12562,7 +12669,7 @@
       <c r="E314"/>
       <c r="H314"/>
     </row>
-    <row r="315" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="315" s="0" customFormat="1" ht="12.75">
       <c r="A315" t="s">
         <v>632</v>
       </c>
@@ -12578,7 +12685,7 @@
       <c r="E315"/>
       <c r="H315"/>
     </row>
-    <row r="316" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="316" s="5" customFormat="1" ht="12.75">
       <c r="A316" t="s">
         <v>632</v>
       </c>
@@ -12594,7 +12701,7 @@
       <c r="E316"/>
       <c r="H316"/>
     </row>
-    <row r="317" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="317" s="0" customFormat="1" ht="12.75">
       <c r="A317" t="s">
         <v>632</v>
       </c>
@@ -12610,7 +12717,7 @@
       <c r="E317"/>
       <c r="H317"/>
     </row>
-    <row r="318" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="318" s="5" customFormat="1" ht="12.75">
       <c r="A318" t="s">
         <v>632</v>
       </c>
@@ -12626,7 +12733,7 @@
       <c r="E318"/>
       <c r="H318"/>
     </row>
-    <row r="319" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="319" s="0" customFormat="1" ht="12.75">
       <c r="A319" t="s">
         <v>632</v>
       </c>
@@ -12642,7 +12749,7 @@
       <c r="E319"/>
       <c r="H319"/>
     </row>
-    <row r="320" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="320" s="5" customFormat="1" ht="12.75">
       <c r="A320" t="s">
         <v>632</v>
       </c>
@@ -12658,7 +12765,7 @@
       <c r="E320"/>
       <c r="H320"/>
     </row>
-    <row r="321" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="321" s="0" customFormat="1" ht="12.75">
       <c r="A321" t="s">
         <v>632</v>
       </c>
@@ -12674,7 +12781,7 @@
       <c r="E321"/>
       <c r="H321"/>
     </row>
-    <row r="322" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="322" s="5" customFormat="1" ht="12.75">
       <c r="A322" t="s">
         <v>632</v>
       </c>
@@ -12690,7 +12797,7 @@
       <c r="E322"/>
       <c r="H322"/>
     </row>
-    <row r="323" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="323" s="0" customFormat="1" ht="12.75">
       <c r="A323" t="s">
         <v>632</v>
       </c>
@@ -12706,7 +12813,7 @@
       <c r="E323"/>
       <c r="H323"/>
     </row>
-    <row r="324" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="324" s="5" customFormat="1" ht="12.75">
       <c r="A324" t="s">
         <v>632</v>
       </c>
@@ -12722,7 +12829,7 @@
       <c r="E324"/>
       <c r="H324"/>
     </row>
-    <row r="325" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="325" s="0" customFormat="1" ht="12.75">
       <c r="A325" t="s">
         <v>632</v>
       </c>
@@ -12738,7 +12845,7 @@
       <c r="E325"/>
       <c r="H325"/>
     </row>
-    <row r="326" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="326" s="5" customFormat="1" ht="12.75">
       <c r="A326" t="s">
         <v>632</v>
       </c>
@@ -12754,7 +12861,7 @@
       <c r="E326"/>
       <c r="H326"/>
     </row>
-    <row r="327" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="327" s="5" customFormat="1" ht="12.75">
       <c r="A327" t="s">
         <v>632</v>
       </c>
@@ -12770,7 +12877,7 @@
       <c r="E327"/>
       <c r="H327"/>
     </row>
-    <row r="328" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="328" s="0" customFormat="1" ht="12.75">
       <c r="A328" t="s">
         <v>632</v>
       </c>
@@ -12784,7 +12891,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="329" s="5" customFormat="1" ht="12.75" hidden="1">
+    <row r="329" s="5" customFormat="1" ht="12.75">
       <c r="A329" t="s">
         <v>632</v>
       </c>
@@ -12800,7 +12907,7 @@
       <c r="E329"/>
       <c r="H329"/>
     </row>
-    <row r="330" s="0" customFormat="1" ht="12.75" hidden="1">
+    <row r="330" s="0" customFormat="1" ht="12.75">
       <c r="A330" t="s">
         <v>632</v>
       </c>
@@ -23696,7 +23803,7 @@
       <c r="E1029"/>
       <c r="H1029"/>
     </row>
-    <row r="1030" ht="12.75" hidden="1">
+    <row r="1030" ht="12.75">
       <c r="A1030" t="s">
         <v>632</v>
       </c>
@@ -23708,7 +23815,7 @@
       </c>
       <c r="D1030"/>
     </row>
-    <row r="1031" ht="12.75" hidden="1">
+    <row r="1031" ht="12.75">
       <c r="A1031" t="s">
         <v>632</v>
       </c>
@@ -23722,7 +23829,7 @@
       <c r="E1031"/>
       <c r="H1031"/>
     </row>
-    <row r="1032" ht="12.75" hidden="1">
+    <row r="1032" ht="12.75">
       <c r="A1032" t="s">
         <v>632</v>
       </c>
@@ -23734,7 +23841,7 @@
       </c>
       <c r="D1032"/>
     </row>
-    <row r="1033" ht="12.75" hidden="1">
+    <row r="1033" ht="12.75">
       <c r="A1033" t="s">
         <v>632</v>
       </c>
@@ -23748,7 +23855,7 @@
       <c r="E1033"/>
       <c r="H1033"/>
     </row>
-    <row r="1034" ht="12.75" hidden="1">
+    <row r="1034" ht="12.75">
       <c r="A1034" t="s">
         <v>632</v>
       </c>
@@ -23760,7 +23867,7 @@
       </c>
       <c r="D1034"/>
     </row>
-    <row r="1035" ht="12.75" hidden="1">
+    <row r="1035" ht="12.75">
       <c r="A1035" t="s">
         <v>632</v>
       </c>
@@ -23774,7 +23881,7 @@
       <c r="E1035"/>
       <c r="H1035"/>
     </row>
-    <row r="1036" ht="12.75" hidden="1">
+    <row r="1036" ht="12.75">
       <c r="A1036" t="s">
         <v>632</v>
       </c>
@@ -23786,7 +23893,7 @@
       </c>
       <c r="D1036"/>
     </row>
-    <row r="1037" ht="12.75" hidden="1">
+    <row r="1037" ht="12.75">
       <c r="A1037" t="s">
         <v>632</v>
       </c>
@@ -23800,7 +23907,7 @@
       <c r="E1037"/>
       <c r="H1037"/>
     </row>
-    <row r="1038" ht="12.75" hidden="1">
+    <row r="1038" ht="12.75">
       <c r="A1038" t="s">
         <v>632</v>
       </c>
@@ -23812,7 +23919,7 @@
       </c>
       <c r="D1038"/>
     </row>
-    <row r="1039" ht="12.75" hidden="1">
+    <row r="1039" ht="12.75">
       <c r="A1039" t="s">
         <v>632</v>
       </c>
@@ -23826,7 +23933,7 @@
       <c r="E1039"/>
       <c r="H1039"/>
     </row>
-    <row r="1040" ht="12.75" hidden="1">
+    <row r="1040" ht="12.75">
       <c r="A1040" t="s">
         <v>632</v>
       </c>
@@ -23838,7 +23945,7 @@
       </c>
       <c r="D1040"/>
     </row>
-    <row r="1041" ht="12.75" hidden="1">
+    <row r="1041" ht="12.75">
       <c r="A1041" t="s">
         <v>632</v>
       </c>
@@ -23852,7 +23959,7 @@
       <c r="E1041"/>
       <c r="H1041"/>
     </row>
-    <row r="1042" ht="12.75" hidden="1">
+    <row r="1042" ht="12.75">
       <c r="A1042" t="s">
         <v>632</v>
       </c>
@@ -23864,7 +23971,7 @@
       </c>
       <c r="D1042"/>
     </row>
-    <row r="1043" ht="12.75" hidden="1">
+    <row r="1043" ht="12.75">
       <c r="A1043" t="s">
         <v>632</v>
       </c>
@@ -23878,7 +23985,7 @@
       <c r="E1043"/>
       <c r="H1043"/>
     </row>
-    <row r="1044" ht="12.75" hidden="1">
+    <row r="1044" ht="12.75">
       <c r="A1044" t="s">
         <v>632</v>
       </c>
@@ -24992,7 +25099,7 @@
       <c r="E1129"/>
       <c r="H1129"/>
     </row>
-    <row r="1130" ht="12.75">
+    <row r="1130" ht="12.75" hidden="1">
       <c r="A1130" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25004,7 +25111,7 @@
       </c>
       <c r="D1130"/>
     </row>
-    <row r="1131" ht="12.75">
+    <row r="1131" ht="12.75" hidden="1">
       <c r="A1131" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25018,7 +25125,7 @@
       <c r="E1131"/>
       <c r="H1131"/>
     </row>
-    <row r="1132" ht="12.75">
+    <row r="1132" ht="12.75" hidden="1">
       <c r="A1132" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25030,7 +25137,7 @@
       </c>
       <c r="D1132"/>
     </row>
-    <row r="1133" ht="12.75">
+    <row r="1133" ht="12.75" hidden="1">
       <c r="A1133" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25044,7 +25151,7 @@
       <c r="E1133"/>
       <c r="H1133"/>
     </row>
-    <row r="1134" ht="12.75">
+    <row r="1134" ht="12.75" hidden="1">
       <c r="A1134" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25056,7 +25163,7 @@
       </c>
       <c r="D1134"/>
     </row>
-    <row r="1135" ht="12.75">
+    <row r="1135" ht="12.75" hidden="1">
       <c r="A1135" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25070,7 +25177,7 @@
       <c r="E1135"/>
       <c r="H1135"/>
     </row>
-    <row r="1136" ht="12.75">
+    <row r="1136" ht="12.75" hidden="1">
       <c r="A1136" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25082,7 +25189,7 @@
       </c>
       <c r="D1136"/>
     </row>
-    <row r="1137" ht="12.75">
+    <row r="1137" ht="12.75" hidden="1">
       <c r="A1137" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25096,7 +25203,7 @@
       <c r="E1137"/>
       <c r="H1137"/>
     </row>
-    <row r="1138" ht="12.75">
+    <row r="1138" ht="12.75" hidden="1">
       <c r="A1138" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25108,7 +25215,7 @@
       </c>
       <c r="D1138"/>
     </row>
-    <row r="1139" ht="12.75">
+    <row r="1139" ht="12.75" hidden="1">
       <c r="A1139" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25122,7 +25229,7 @@
       <c r="E1139"/>
       <c r="H1139"/>
     </row>
-    <row r="1140" ht="12.75">
+    <row r="1140" ht="12.75" hidden="1">
       <c r="A1140" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25134,7 +25241,7 @@
       </c>
       <c r="D1140"/>
     </row>
-    <row r="1141" ht="12.75">
+    <row r="1141" ht="12.75" hidden="1">
       <c r="A1141" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25148,7 +25255,7 @@
       <c r="E1141"/>
       <c r="H1141"/>
     </row>
-    <row r="1142" ht="12.75">
+    <row r="1142" ht="12.75" hidden="1">
       <c r="A1142" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25160,7 +25267,7 @@
       </c>
       <c r="D1142"/>
     </row>
-    <row r="1143" ht="12.75">
+    <row r="1143" ht="12.75" hidden="1">
       <c r="A1143" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25174,7 +25281,7 @@
       <c r="E1143"/>
       <c r="H1143"/>
     </row>
-    <row r="1144" ht="12.75">
+    <row r="1144" ht="12.75" hidden="1">
       <c r="A1144" s="7" t="s">
         <v>2218</v>
       </c>
@@ -25186,7 +25293,7 @@
       </c>
       <c r="D1144"/>
     </row>
-    <row r="1145" ht="12.75">
+    <row r="1145" ht="12.75" hidden="1">
       <c r="A1145" s="7" t="s">
         <v>2218</v>
       </c>
@@ -26065,7 +26172,7 @@
       <c r="B1212" t="s">
         <v>2303</v>
       </c>
-      <c r="C1212" s="11" t="s">
+      <c r="C1212" s="8" t="s">
         <v>2304</v>
       </c>
       <c r="D1212"/>
@@ -26096,7 +26203,7 @@
       </c>
       <c r="D1214"/>
     </row>
-    <row r="1215" ht="12.75">
+    <row r="1215" ht="12.75" hidden="1">
       <c r="A1215" s="7" t="s">
         <v>2218</v>
       </c>
@@ -26111,135 +26218,249 @@
       <c r="H1215"/>
     </row>
     <row r="1216" ht="12.75">
-      <c r="A1216"/>
-      <c r="B1216"/>
-      <c r="C1216"/>
+      <c r="A1216" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1216" t="s">
+        <v>2309</v>
+      </c>
+      <c r="C1216" t="s">
+        <v>2310</v>
+      </c>
       <c r="D1216"/>
     </row>
     <row r="1217" ht="12.75">
-      <c r="A1217"/>
-      <c r="B1217"/>
-      <c r="C1217"/>
+      <c r="A1217" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1217" t="s">
+        <v>2311</v>
+      </c>
+      <c r="C1217" t="s">
+        <v>2312</v>
+      </c>
       <c r="D1217"/>
       <c r="E1217"/>
       <c r="H1217"/>
     </row>
     <row r="1218" ht="12.75">
-      <c r="A1218"/>
-      <c r="B1218"/>
-      <c r="C1218"/>
+      <c r="A1218" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1218" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C1218" t="s">
+        <v>2314</v>
+      </c>
       <c r="D1218"/>
     </row>
     <row r="1219" ht="12.75">
-      <c r="A1219"/>
-      <c r="B1219"/>
-      <c r="C1219"/>
+      <c r="A1219" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C1219" t="s">
+        <v>2316</v>
+      </c>
       <c r="D1219"/>
       <c r="E1219"/>
       <c r="H1219"/>
     </row>
     <row r="1220" ht="12.75">
-      <c r="A1220"/>
-      <c r="B1220"/>
-      <c r="C1220"/>
+      <c r="A1220" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>2317</v>
+      </c>
+      <c r="C1220" t="s">
+        <v>1130</v>
+      </c>
       <c r="D1220"/>
     </row>
     <row r="1221" ht="12.75">
-      <c r="A1221"/>
-      <c r="B1221"/>
-      <c r="C1221"/>
+      <c r="A1221" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>2318</v>
+      </c>
+      <c r="C1221" t="s">
+        <v>2319</v>
+      </c>
       <c r="D1221"/>
       <c r="E1221"/>
       <c r="H1221"/>
     </row>
     <row r="1222" ht="12.75">
-      <c r="A1222"/>
-      <c r="B1222"/>
-      <c r="C1222"/>
+      <c r="A1222" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>2320</v>
+      </c>
+      <c r="C1222" t="s">
+        <v>2321</v>
+      </c>
       <c r="D1222"/>
     </row>
     <row r="1223" ht="12.75">
-      <c r="A1223"/>
-      <c r="B1223"/>
-      <c r="C1223"/>
+      <c r="A1223" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1223" t="s">
+        <v>2323</v>
+      </c>
       <c r="D1223"/>
       <c r="E1223"/>
       <c r="H1223"/>
     </row>
     <row r="1224" ht="12.75">
-      <c r="A1224"/>
-      <c r="B1224"/>
-      <c r="C1224"/>
+      <c r="A1224" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>2324</v>
+      </c>
+      <c r="C1224" t="s">
+        <v>2325</v>
+      </c>
       <c r="D1224"/>
     </row>
     <row r="1225" ht="12.75">
-      <c r="A1225"/>
-      <c r="B1225"/>
-      <c r="C1225"/>
+      <c r="A1225" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1225" t="s">
+        <v>2326</v>
+      </c>
+      <c r="C1225" t="s">
+        <v>2327</v>
+      </c>
       <c r="D1225"/>
       <c r="E1225"/>
       <c r="H1225"/>
     </row>
     <row r="1226" ht="12.75">
-      <c r="A1226"/>
-      <c r="B1226"/>
-      <c r="C1226"/>
+      <c r="A1226" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1226" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C1226" t="s">
+        <v>1130</v>
+      </c>
       <c r="D1226"/>
     </row>
     <row r="1227" ht="12.75">
-      <c r="A1227"/>
-      <c r="B1227"/>
-      <c r="C1227"/>
+      <c r="A1227" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1227" t="s">
+        <v>2329</v>
+      </c>
+      <c r="C1227" t="s">
+        <v>2330</v>
+      </c>
       <c r="D1227"/>
       <c r="E1227"/>
       <c r="H1227"/>
     </row>
     <row r="1228" ht="12.75">
-      <c r="A1228"/>
-      <c r="B1228"/>
-      <c r="C1228"/>
+      <c r="A1228" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1228" t="s">
+        <v>2331</v>
+      </c>
+      <c r="C1228" t="s">
+        <v>2332</v>
+      </c>
       <c r="D1228"/>
     </row>
     <row r="1229" ht="12.75">
-      <c r="A1229"/>
-      <c r="B1229"/>
-      <c r="C1229"/>
+      <c r="A1229" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1229" t="s">
+        <v>2333</v>
+      </c>
+      <c r="C1229" t="s">
+        <v>2334</v>
+      </c>
       <c r="D1229"/>
       <c r="E1229"/>
       <c r="H1229"/>
     </row>
     <row r="1230" ht="12.75">
-      <c r="A1230"/>
-      <c r="B1230"/>
-      <c r="C1230"/>
+      <c r="A1230" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1230" s="11">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="C1230" t="s">
+        <v>2335</v>
+      </c>
       <c r="D1230"/>
     </row>
     <row r="1231" ht="12.75">
-      <c r="A1231"/>
-      <c r="B1231"/>
-      <c r="C1231"/>
+      <c r="A1231" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1231" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C1231" t="s">
+        <v>2337</v>
+      </c>
       <c r="D1231"/>
       <c r="E1231"/>
       <c r="H1231"/>
     </row>
     <row r="1232" ht="12.75">
-      <c r="A1232"/>
-      <c r="B1232"/>
-      <c r="C1232"/>
+      <c r="A1232" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1232" t="s">
+        <v>2338</v>
+      </c>
+      <c r="C1232" t="s">
+        <v>403</v>
+      </c>
       <c r="D1232"/>
     </row>
     <row r="1233" ht="12.75">
-      <c r="A1233"/>
-      <c r="B1233"/>
-      <c r="C1233"/>
+      <c r="A1233" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1233" t="s">
+        <v>2339</v>
+      </c>
+      <c r="C1233" t="s">
+        <v>2340</v>
+      </c>
       <c r="D1233"/>
       <c r="E1233"/>
       <c r="H1233"/>
     </row>
     <row r="1234" ht="12.75">
-      <c r="A1234"/>
-      <c r="B1234"/>
-      <c r="C1234"/>
+      <c r="A1234" s="7" t="s">
+        <v>2308</v>
+      </c>
+      <c r="B1234" t="s">
+        <v>2341</v>
+      </c>
+      <c r="C1234" t="s">
+        <v>2342</v>
+      </c>
       <c r="D1234"/>
     </row>
     <row r="1235" ht="12.75">
@@ -29198,10 +29419,10 @@
       <c r="C2651" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1214">
+  <autoFilter ref="A1:D1215">
     <filterColumn colId="0">
       <filters>
-        <filter val="(This is ...) MFDOOM"/>
+        <filter val="Brazilian CityPop"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>